<commit_message>
Added computation of Standard Deviation
</commit_message>
<xml_diff>
--- a/eth-gas/data/ETH_EUR.xlsx
+++ b/eth-gas/data/ETH_EUR.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\QuickTest\zkConsent\zkconsent\eth-gas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50531186-DD91-4C4E-894C-D1F72E214054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A19E6D-7891-4B53-A352-3B70756A9A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ETH_EUR" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Source</t>
   </si>
@@ -155,12 +167,18 @@
   </si>
   <si>
     <t>Median Lo</t>
+  </si>
+  <si>
+    <t>Standard Deviation Hi</t>
+  </si>
+  <si>
+    <t>Standard Deviation Lo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -995,11 +1013,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,11 +1029,12 @@
     <col min="5" max="5" width="19.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1046,7 +1065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1076,7 +1095,7 @@
         <v>3497.82</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1106,7 +1125,7 @@
         <v>4301.99</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1136,7 +1155,7 @@
         <v>3995.8216666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1166,7 +1185,7 @@
         <v>3965.8900000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1189,67 +1208,78 @@
         <v>426024238686</v>
       </c>
       <c r="J7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="1">
+        <f>_xlfn.STDEV.P(C3:C32)</f>
+        <v>155.03462591914399</v>
+      </c>
+      <c r="L7" s="1">
+        <f>_xlfn.STDEV.S(C3:C32)</f>
+        <v>157.68498244991468</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3812.22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4061.34</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3792.92</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3815.21</v>
+      </c>
+      <c r="F8" s="1">
+        <v>16694532299</v>
+      </c>
+      <c r="G8" s="1">
+        <v>452026824418</v>
+      </c>
+      <c r="J8" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K8" s="1">
         <f>AVERAGE(D:D)</f>
         <v>3766.2106666666664</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3812.22</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4061.34</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3792.92</v>
-      </c>
-      <c r="E8" s="1">
-        <v>3815.21</v>
-      </c>
-      <c r="F8" s="1">
-        <v>16694532299</v>
-      </c>
-      <c r="G8" s="1">
-        <v>452026824418</v>
-      </c>
-      <c r="J8" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3858.86</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3891.62</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3713.17</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3769.9</v>
+      </c>
+      <c r="F9" s="1">
+        <v>19416875790</v>
+      </c>
+      <c r="G9" s="1">
+        <v>446597258313</v>
+      </c>
+      <c r="J9" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K9" s="1">
         <f>MEDIAN(D:D)</f>
         <v>3781.5550000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3858.86</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3891.62</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3713.17</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3769.9</v>
-      </c>
-      <c r="F9" s="1">
-        <v>19416875790</v>
-      </c>
-      <c r="G9" s="1">
-        <v>446597258313</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1271,8 +1301,19 @@
       <c r="G10" s="1">
         <v>457430298778</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="1">
+        <f>_xlfn.STDEV.P(D3:D32)</f>
+        <v>168.27900397719131</v>
+      </c>
+      <c r="L10" s="1">
+        <f>_xlfn.STDEV.S(D3:D32)</f>
+        <v>171.15577653389192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1295,7 +1336,7 @@
         <v>429301263929</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1318,7 +1359,7 @@
         <v>448024912696</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1341,7 +1382,7 @@
         <v>462684120561</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1364,7 +1405,7 @@
         <v>447654193841</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1387,7 +1428,7 @@
         <v>418463046442</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>

</xml_diff>